<commit_message>
updated cost estimation, product description, updated schedule, and added hour estimation.
</commit_message>
<xml_diff>
--- a/Project_Reports/Tables/schedule_visualized.xlsx
+++ b/Project_Reports/Tables/schedule_visualized.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UND\Classes\CSCI_463\CSCI-463-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdres\OneDrive\Desktop\CSCI-463-Project\Project_Reports\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6F6B16-E254-4AB3-8F0F-B5EC12A53381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{0F6F6B16-E254-4AB3-8F0F-B5EC12A53381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F96758D3-15DF-40DA-8D69-E9C677606637}"/>
   <bookViews>
-    <workbookView xWindow="-18915" yWindow="1350" windowWidth="28800" windowHeight="15435" xr2:uid="{B6595D73-F54C-4286-8E95-AB76305C48C5}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="15435" xr2:uid="{B6595D73-F54C-4286-8E95-AB76305C48C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>January</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>23rd</t>
+  </si>
+  <si>
+    <t>Continuous Software Design, Implementation, and Testing</t>
+  </si>
+  <si>
+    <t>18th</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -258,76 +270,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -647,311 +669,314 @@
   <dimension ref="D1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="16" t="s">
+      <c r="N1" s="22"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="I2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="M2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="15" t="s">
+      <c r="N2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="19"/>
-      <c r="S2" s="21" t="s">
+      <c r="R2" s="11"/>
+      <c r="S2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
     </row>
     <row r="4" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="25" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="25" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="25" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="25" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="12"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
     </row>
     <row r="8" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="26" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="27"/>
+    </row>
+    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="19"/>
-      <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
     </row>
     <row r="11" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="Q8:R8"/>
+  <mergeCells count="13">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G8:R8"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="Q9:R9"/>
     <mergeCell ref="O7:S7"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>